<commit_message>
removes subsite and run columns from release metadata and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/release-metadata.xlsx
+++ b/data-raw/metadata/release-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270C884-C5F7-0E48-AB85-A75B8E100532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77070596-1E8B-DA44-A586-ACB18E9BC6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -194,18 +194,6 @@
   </si>
   <si>
     <t>hh:mm:ss</t>
-  </si>
-  <si>
-    <t>subsite</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>Subsite of released fish.</t>
-  </si>
-  <si>
-    <t>Run identified of the fish.</t>
   </si>
   <si>
     <t>2003-12-03</t>
@@ -667,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,7 +755,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>54</v>
@@ -793,10 +781,10 @@
         <v>55</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -804,7 +792,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -935,7 +923,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>37</v>
@@ -1049,7 +1037,7 @@
         <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -1061,55 +1049,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1021 C1:C6" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1019" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E1021 E1:E6" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1019" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F1021 F1:F6" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1019" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1048576 H1:H6" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{0E975802-AAEB-481A-9F6C-1EEB8BBDECAC}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>